<commit_message>
Функции conver_in_datetime и update_pm_db
1 Обновил json PM и Students по формату присланному от Тима. В pm.json добавил поле "work_time" для тестирования
2 В Models tg_id добавил в необязательное поле для заполнения при создании записи
3 В Main при открытии json указал кодировку, на Win была проблема
4 Добавил функцию conver_in_datetime
5 Обновил функцию update_pm_db с применением conver_in_datetime
6 Добавил тестовую функцию set_work_time_pm_db - заполняет поля времени таблицы PM из json
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -633,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -772,8 +772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>